<commit_message>
updated the report, can be found in project3-><Microsoft doc>
</commit_message>
<xml_diff>
--- a/Project3/Proj_3_Comparisons.xlsx
+++ b/Project3/Proj_3_Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8d6d17d704a0d79/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{8FD10B32-5967-4EF2-8415-9FF12EF4BCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDF286A6-E6A8-4ADD-BCEE-8D089187656C}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{8FD10B32-5967-4EF2-8415-9FF12EF4BCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DC28A52-3559-404B-A4E2-982F862C21FF}"/>
   <bookViews>
-    <workbookView xWindow="38805" yWindow="-16515" windowWidth="29040" windowHeight="15720" xr2:uid="{872E82F7-91BA-41D7-8E7A-6C9894B04642}"/>
+    <workbookView xWindow="50910" yWindow="-16395" windowWidth="16920" windowHeight="15585" xr2:uid="{872E82F7-91BA-41D7-8E7A-6C9894B04642}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Benchmark</t>
   </si>
@@ -63,6 +63,57 @@
   </si>
   <si>
     <t># Instructions</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>Max Cycle Time</t>
+  </si>
+  <si>
+    <t>Total Execution time</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>2.11</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>47.39mhz</t>
+  </si>
+  <si>
+    <t>53.02mhz</t>
+  </si>
+  <si>
+    <t>24.74mhz</t>
+  </si>
+  <si>
+    <t>85,529.5ns</t>
+  </si>
+  <si>
+    <t>33,427.6ns</t>
+  </si>
+  <si>
+    <t>114,843ns</t>
+  </si>
+  <si>
+    <t>45,662ns</t>
+  </si>
+  <si>
+    <t>94091.6ns</t>
+  </si>
+  <si>
+    <t>39375.4ns</t>
   </si>
 </sst>
 </file>
@@ -172,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,19 +262,80 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -293,7 +405,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -316,10 +428,33 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -334,14 +469,21 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B13042-1C27-448E-B78F-3A9DA4F3FB99}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="A1:D7" xr:uid="{D0B13042-1C27-448E-B78F-3A9DA4F3FB99}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D36D29A3-4C54-44BC-B0A7-A094C97F47F2}" name="Processor" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6761F22A-E02C-400D-86CE-56E0B1BC3F6A}" name="Benchmark" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{6ECF179E-8A49-4EA7-95B1-9D24610ADBF2}" name="# Instructions" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D0577C32-7697-48C3-AC63-95C3C0043E2E}" name="Total Cycles To Execute" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B13042-1C27-448E-B78F-3A9DA4F3FB99}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G7" xr:uid="{D0B13042-1C27-448E-B78F-3A9DA4F3FB99}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D36D29A3-4C54-44BC-B0A7-A094C97F47F2}" name="Processor" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6761F22A-E02C-400D-86CE-56E0B1BC3F6A}" name="Benchmark" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6ECF179E-8A49-4EA7-95B1-9D24610ADBF2}" name="# Instructions" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D0577C32-7697-48C3-AC63-95C3C0043E2E}" name="Total Cycles To Execute" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AAEC3EA0-5C21-41BA-8BF1-76A34EC0A6B9}" name="CPI" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{0C6C31D8-5049-4717-919D-93B5358E98B0}" name="Max Cycle Time" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{9626AC02-6C9B-488A-A196-A536DB41CF87}" name="Total Execution time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -667,15 +809,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24.53125" customWidth="1"/>
     <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" customWidth="1"/>
+    <col min="6" max="6" width="18.3984375" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -691,6 +836,15 @@
       <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
@@ -705,8 +859,15 @@
       <c r="D2" s="4">
         <v>2116</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="E2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="11"/>
@@ -719,6 +880,13 @@
       <c r="D3" s="13">
         <v>827</v>
       </c>
+      <c r="E3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
@@ -732,6 +900,15 @@
       </c>
       <c r="D4" s="5">
         <v>6089</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -745,6 +922,13 @@
       <c r="D5" s="5">
         <v>2421</v>
       </c>
+      <c r="E5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
@@ -756,8 +940,17 @@
       <c r="C6" s="6">
         <v>2116</v>
       </c>
-      <c r="D6" s="15">
-        <v>4887</v>
+      <c r="D6" s="14">
+        <v>4459</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -765,11 +958,18 @@
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>827</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>1866</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>